<commit_message>
created verbose version opf fine mapping
</commit_message>
<xml_diff>
--- a/tables_plots/phenotype_statistics.xlsx
+++ b/tables_plots/phenotype_statistics.xlsx
@@ -499,16 +499,16 @@
         <v>8.208149316467916</v>
       </c>
       <c r="F2" t="n">
+        <v>43.04335090802577</v>
+      </c>
+      <c r="G2" t="n">
         <v>56.95664909197422</v>
       </c>
-      <c r="G2" t="n">
-        <v>43.04335090802577</v>
-      </c>
       <c r="H2" t="n">
+        <v>46.22967718008432</v>
+      </c>
+      <c r="I2" t="n">
         <v>53.77032281991568</v>
-      </c>
-      <c r="I2" t="n">
-        <v>46.22967718008432</v>
       </c>
     </row>
     <row r="3">
@@ -530,16 +530,16 @@
         <v>8.197679226263878</v>
       </c>
       <c r="F3" t="n">
+        <v>56.79158093567646</v>
+      </c>
+      <c r="G3" t="n">
         <v>43.20841906432354</v>
       </c>
-      <c r="G3" t="n">
-        <v>56.79158093567646</v>
-      </c>
       <c r="H3" t="n">
+        <v>43.96685140646241</v>
+      </c>
+      <c r="I3" t="n">
         <v>56.0331485935376</v>
-      </c>
-      <c r="I3" t="n">
-        <v>43.96685140646241</v>
       </c>
     </row>
     <row r="4">
@@ -561,16 +561,16 @@
         <v>8.126561179821776</v>
       </c>
       <c r="F4" t="n">
+        <v>43.45208522079668</v>
+      </c>
+      <c r="G4" t="n">
         <v>56.54791477920332</v>
       </c>
-      <c r="G4" t="n">
-        <v>43.45208522079668</v>
-      </c>
       <c r="H4" t="n">
+        <v>45.87570566024775</v>
+      </c>
+      <c r="I4" t="n">
         <v>54.12429433975225</v>
-      </c>
-      <c r="I4" t="n">
-        <v>45.87570566024775</v>
       </c>
     </row>
     <row r="5">
@@ -592,16 +592,16 @@
         <v>8.155195943858121</v>
       </c>
       <c r="F5" t="n">
+        <v>53.29466101610011</v>
+      </c>
+      <c r="G5" t="n">
         <v>46.70533898389989</v>
       </c>
-      <c r="G5" t="n">
-        <v>53.29466101610011</v>
-      </c>
       <c r="H5" t="n">
+        <v>43.46800155555101</v>
+      </c>
+      <c r="I5" t="n">
         <v>56.53199844444899</v>
-      </c>
-      <c r="I5" t="n">
-        <v>43.46800155555101</v>
       </c>
     </row>
     <row r="6">
@@ -623,16 +623,16 @@
         <v>8.160469286963792</v>
       </c>
       <c r="F6" t="n">
+        <v>75.89955849889624</v>
+      </c>
+      <c r="G6" t="n">
         <v>24.10044150110375</v>
       </c>
-      <c r="G6" t="n">
-        <v>75.89955849889624</v>
-      </c>
       <c r="H6" t="n">
+        <v>44.39595557170977</v>
+      </c>
+      <c r="I6" t="n">
         <v>55.60404442829024</v>
-      </c>
-      <c r="I6" t="n">
-        <v>44.39595557170977</v>
       </c>
     </row>
     <row r="7">
@@ -654,16 +654,16 @@
         <v>8.186824556550057</v>
       </c>
       <c r="F7" t="n">
+        <v>46.27117035912519</v>
+      </c>
+      <c r="G7" t="n">
         <v>53.72882964087481</v>
       </c>
-      <c r="G7" t="n">
-        <v>46.27117035912519</v>
-      </c>
       <c r="H7" t="n">
+        <v>45.6264887803511</v>
+      </c>
+      <c r="I7" t="n">
         <v>54.3735112196489</v>
-      </c>
-      <c r="I7" t="n">
-        <v>45.6264887803511</v>
       </c>
     </row>
     <row r="8">
@@ -685,16 +685,16 @@
         <v>8.234033347455275</v>
       </c>
       <c r="F8" t="n">
+        <v>0.04038270377733599</v>
+      </c>
+      <c r="G8" t="n">
         <v>99.95961729622267</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.04038270377733599</v>
-      </c>
       <c r="H8" t="n">
+        <v>49.27542954235856</v>
+      </c>
+      <c r="I8" t="n">
         <v>50.72457045764144</v>
-      </c>
-      <c r="I8" t="n">
-        <v>49.27542954235856</v>
       </c>
     </row>
     <row r="9">
@@ -716,16 +716,16 @@
         <v>8.167825341006401</v>
       </c>
       <c r="F9" t="n">
+        <v>30.70993280900047</v>
+      </c>
+      <c r="G9" t="n">
         <v>69.29006719099952</v>
       </c>
-      <c r="G9" t="n">
-        <v>30.70993280900047</v>
-      </c>
       <c r="H9" t="n">
+        <v>46.3684440921406</v>
+      </c>
+      <c r="I9" t="n">
         <v>53.63155590785939</v>
-      </c>
-      <c r="I9" t="n">
-        <v>46.3684440921406</v>
       </c>
     </row>
     <row r="10">
@@ -747,16 +747,16 @@
         <v>8.1871440231343</v>
       </c>
       <c r="F10" t="n">
+        <v>42.97319048337609</v>
+      </c>
+      <c r="G10" t="n">
         <v>57.02680951662391</v>
       </c>
-      <c r="G10" t="n">
-        <v>42.97319048337609</v>
-      </c>
       <c r="H10" t="n">
+        <v>45.95649318993564</v>
+      </c>
+      <c r="I10" t="n">
         <v>54.04350681006436</v>
-      </c>
-      <c r="I10" t="n">
-        <v>45.95649318993564</v>
       </c>
     </row>
     <row r="11">
@@ -778,16 +778,16 @@
         <v>8.154128243626934</v>
       </c>
       <c r="F11" t="n">
+        <v>38.74272769397106</v>
+      </c>
+      <c r="G11" t="n">
         <v>61.25727230602893</v>
       </c>
-      <c r="G11" t="n">
-        <v>38.74272769397106</v>
-      </c>
       <c r="H11" t="n">
+        <v>46.00737231617151</v>
+      </c>
+      <c r="I11" t="n">
         <v>53.99262768382849</v>
-      </c>
-      <c r="I11" t="n">
-        <v>46.00737231617151</v>
       </c>
     </row>
     <row r="12">
@@ -809,16 +809,16 @@
         <v>8.141639666945164</v>
       </c>
       <c r="F12" t="n">
+        <v>0.03080596095344449</v>
+      </c>
+      <c r="G12" t="n">
         <v>99.96919403904656</v>
       </c>
-      <c r="G12" t="n">
-        <v>0.03080596095344449</v>
-      </c>
       <c r="H12" t="n">
+        <v>48.53923938005747</v>
+      </c>
+      <c r="I12" t="n">
         <v>51.46076061994253</v>
-      </c>
-      <c r="I12" t="n">
-        <v>48.53923938005747</v>
       </c>
     </row>
     <row r="13">
@@ -840,16 +840,16 @@
         <v>8.195636853068622</v>
       </c>
       <c r="F13" t="n">
+        <v>45.34216753431141</v>
+      </c>
+      <c r="G13" t="n">
         <v>54.65783246568859</v>
       </c>
-      <c r="G13" t="n">
-        <v>45.34216753431141</v>
-      </c>
       <c r="H13" t="n">
+        <v>45.73496936931378</v>
+      </c>
+      <c r="I13" t="n">
         <v>54.26503063068622</v>
-      </c>
-      <c r="I13" t="n">
-        <v>45.73496936931378</v>
       </c>
     </row>
     <row r="14">
@@ -871,16 +871,16 @@
         <v>8.170830695373516</v>
       </c>
       <c r="F14" t="n">
+        <v>36.73271173271173</v>
+      </c>
+      <c r="G14" t="n">
         <v>63.26728826728827</v>
       </c>
-      <c r="G14" t="n">
-        <v>36.73271173271173</v>
-      </c>
       <c r="H14" t="n">
+        <v>46.01238361047916</v>
+      </c>
+      <c r="I14" t="n">
         <v>53.98761638952084</v>
-      </c>
-      <c r="I14" t="n">
-        <v>46.01238361047916</v>
       </c>
     </row>
     <row r="15">
@@ -902,16 +902,16 @@
         <v>8.173838546030904</v>
       </c>
       <c r="F15" t="n">
+        <v>28.57498961362692</v>
+      </c>
+      <c r="G15" t="n">
         <v>71.42501038637307</v>
       </c>
-      <c r="G15" t="n">
-        <v>28.57498961362692</v>
-      </c>
       <c r="H15" t="n">
+        <v>46.67403960320196</v>
+      </c>
+      <c r="I15" t="n">
         <v>53.32596039679805</v>
-      </c>
-      <c r="I15" t="n">
-        <v>46.67403960320196</v>
       </c>
     </row>
     <row r="16">
@@ -933,16 +933,16 @@
         <v>8.181792133759497</v>
       </c>
       <c r="F16" t="n">
+        <v>45.15285326086956</v>
+      </c>
+      <c r="G16" t="n">
         <v>54.84714673913044</v>
       </c>
-      <c r="G16" t="n">
-        <v>45.15285326086956</v>
-      </c>
       <c r="H16" t="n">
+        <v>45.72620970284256</v>
+      </c>
+      <c r="I16" t="n">
         <v>54.27379029715743</v>
-      </c>
-      <c r="I16" t="n">
-        <v>45.72620970284256</v>
       </c>
     </row>
     <row r="17">
@@ -964,16 +964,16 @@
         <v>8.15978050404031</v>
       </c>
       <c r="F17" t="n">
+        <v>99.96037337090526</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.03962662909475168</v>
       </c>
-      <c r="G17" t="n">
-        <v>99.96037337090526</v>
-      </c>
       <c r="H17" t="n">
+        <v>42.74687307624397</v>
+      </c>
+      <c r="I17" t="n">
         <v>57.25312692375603</v>
-      </c>
-      <c r="I17" t="n">
-        <v>42.74687307624397</v>
       </c>
     </row>
     <row r="18">
@@ -995,16 +995,16 @@
         <v>8.172336721337651</v>
       </c>
       <c r="F18" t="n">
+        <v>52.47528709600064</v>
+      </c>
+      <c r="G18" t="n">
         <v>47.52471290399936</v>
       </c>
-      <c r="G18" t="n">
-        <v>52.47528709600064</v>
-      </c>
       <c r="H18" t="n">
+        <v>42.19479584490384</v>
+      </c>
+      <c r="I18" t="n">
         <v>57.80520415509617</v>
-      </c>
-      <c r="I18" t="n">
-        <v>42.19479584490384</v>
       </c>
     </row>
     <row r="19">
@@ -1026,16 +1026,16 @@
         <v>8.149631350820437</v>
       </c>
       <c r="F19" t="n">
+        <v>31.60560177768591</v>
+      </c>
+      <c r="G19" t="n">
         <v>68.39439822231409</v>
       </c>
-      <c r="G19" t="n">
-        <v>31.60560177768591</v>
-      </c>
       <c r="H19" t="n">
+        <v>46.33305165186064</v>
+      </c>
+      <c r="I19" t="n">
         <v>53.66694834813936</v>
-      </c>
-      <c r="I19" t="n">
-        <v>46.33305165186064</v>
       </c>
     </row>
     <row r="20">
@@ -1057,16 +1057,16 @@
         <v>8.164282360888011</v>
       </c>
       <c r="F20" t="n">
+        <v>49.46977730646871</v>
+      </c>
+      <c r="G20" t="n">
         <v>50.53022269353128</v>
       </c>
-      <c r="G20" t="n">
-        <v>49.46977730646871</v>
-      </c>
       <c r="H20" t="n">
+        <v>45.42928584556157</v>
+      </c>
+      <c r="I20" t="n">
         <v>54.57071415443843</v>
-      </c>
-      <c r="I20" t="n">
-        <v>45.42928584556157</v>
       </c>
     </row>
     <row r="21">
@@ -1088,16 +1088,16 @@
         <v>8.183335318479008</v>
       </c>
       <c r="F21" t="n">
+        <v>46.1186768049681</v>
+      </c>
+      <c r="G21" t="n">
         <v>53.8813231950319</v>
       </c>
-      <c r="G21" t="n">
-        <v>46.1186768049681</v>
-      </c>
       <c r="H21" t="n">
+        <v>45.6440674161227</v>
+      </c>
+      <c r="I21" t="n">
         <v>54.3559325838773</v>
-      </c>
-      <c r="I21" t="n">
-        <v>45.6440674161227</v>
       </c>
     </row>
     <row r="22">
@@ -1119,16 +1119,16 @@
         <v>8.181354872306718</v>
       </c>
       <c r="F22" t="n">
+        <v>37.32303242502664</v>
+      </c>
+      <c r="G22" t="n">
         <v>62.67696757497336</v>
       </c>
-      <c r="G22" t="n">
-        <v>37.32303242502664</v>
-      </c>
       <c r="H22" t="n">
+        <v>46.21695248088021</v>
+      </c>
+      <c r="I22" t="n">
         <v>53.78304751911978</v>
-      </c>
-      <c r="I22" t="n">
-        <v>46.21695248088021</v>
       </c>
     </row>
     <row r="23">
@@ -1150,16 +1150,16 @@
         <v>8.165534911739867</v>
       </c>
       <c r="F23" t="n">
+        <v>44.07839661200571</v>
+      </c>
+      <c r="G23" t="n">
         <v>55.92160338799429</v>
       </c>
-      <c r="G23" t="n">
-        <v>44.07839661200571</v>
-      </c>
       <c r="H23" t="n">
+        <v>45.76555075004686</v>
+      </c>
+      <c r="I23" t="n">
         <v>54.23444924995314</v>
-      </c>
-      <c r="I23" t="n">
-        <v>45.76555075004686</v>
       </c>
     </row>
     <row r="24">
@@ -1181,16 +1181,16 @@
         <v>8.186363105183252</v>
       </c>
       <c r="F24" t="n">
+        <v>17.85390199637024</v>
+      </c>
+      <c r="G24" t="n">
         <v>82.14609800362976</v>
       </c>
-      <c r="G24" t="n">
-        <v>17.85390199637024</v>
-      </c>
       <c r="H24" t="n">
+        <v>46.84498635019874</v>
+      </c>
+      <c r="I24" t="n">
         <v>53.15501364980126</v>
-      </c>
-      <c r="I24" t="n">
-        <v>46.84498635019874</v>
       </c>
     </row>
     <row r="25">
@@ -1212,16 +1212,16 @@
         <v>8.22876568830972</v>
       </c>
       <c r="F25" t="n">
+        <v>43.79021411748363</v>
+      </c>
+      <c r="G25" t="n">
         <v>56.20978588251637</v>
       </c>
-      <c r="G25" t="n">
-        <v>43.79021411748363</v>
-      </c>
       <c r="H25" t="n">
+        <v>46.74837621673493</v>
+      </c>
+      <c r="I25" t="n">
         <v>53.25162378326507</v>
-      </c>
-      <c r="I25" t="n">
-        <v>46.74837621673493</v>
       </c>
     </row>
     <row r="26">
@@ -1243,16 +1243,16 @@
         <v>8.184845491873718</v>
       </c>
       <c r="F26" t="n">
+        <v>43.773565678182</v>
+      </c>
+      <c r="G26" t="n">
         <v>56.226434321818</v>
       </c>
-      <c r="G26" t="n">
-        <v>43.773565678182</v>
-      </c>
       <c r="H26" t="n">
+        <v>45.87467272122058</v>
+      </c>
+      <c r="I26" t="n">
         <v>54.12532727877942</v>
-      </c>
-      <c r="I26" t="n">
-        <v>45.87467272122058</v>
       </c>
     </row>
     <row r="27">
@@ -1274,16 +1274,16 @@
         <v>8.156411058383776</v>
       </c>
       <c r="F27" t="n">
+        <v>54.5391954362152</v>
+      </c>
+      <c r="G27" t="n">
         <v>45.4608045637848</v>
       </c>
-      <c r="G27" t="n">
-        <v>54.5391954362152</v>
-      </c>
       <c r="H27" t="n">
+        <v>45.26098510012338</v>
+      </c>
+      <c r="I27" t="n">
         <v>54.73901489987662</v>
-      </c>
-      <c r="I27" t="n">
-        <v>45.26098510012338</v>
       </c>
     </row>
     <row r="28">
@@ -1305,16 +1305,16 @@
         <v>8.164237815013115</v>
       </c>
       <c r="F28" t="n">
+        <v>47.07479000843634</v>
+      </c>
+      <c r="G28" t="n">
         <v>52.92520999156366</v>
       </c>
-      <c r="G28" t="n">
-        <v>47.07479000843634</v>
-      </c>
       <c r="H28" t="n">
+        <v>45.23353027088429</v>
+      </c>
+      <c r="I28" t="n">
         <v>54.76646972911571</v>
-      </c>
-      <c r="I28" t="n">
-        <v>45.23353027088429</v>
       </c>
     </row>
     <row r="29">
@@ -1336,16 +1336,16 @@
         <v>8.166424221183339</v>
       </c>
       <c r="F29" t="n">
+        <v>91.82029107783168</v>
+      </c>
+      <c r="G29" t="n">
         <v>8.179708922168318</v>
       </c>
-      <c r="G29" t="n">
-        <v>91.82029107783168</v>
-      </c>
       <c r="H29" t="n">
+        <v>43.07250023319278</v>
+      </c>
+      <c r="I29" t="n">
         <v>56.92749976680722</v>
-      </c>
-      <c r="I29" t="n">
-        <v>43.07250023319278</v>
       </c>
     </row>
     <row r="30">
@@ -1367,16 +1367,16 @@
         <v>8.160718734205309</v>
       </c>
       <c r="F30" t="n">
+        <v>64.61732423613171</v>
+      </c>
+      <c r="G30" t="n">
         <v>35.38267576386828</v>
       </c>
-      <c r="G30" t="n">
-        <v>64.61732423613171</v>
-      </c>
       <c r="H30" t="n">
+        <v>44.45746132299696</v>
+      </c>
+      <c r="I30" t="n">
         <v>55.54253867700303</v>
-      </c>
-      <c r="I30" t="n">
-        <v>44.45746132299696</v>
       </c>
     </row>
     <row r="31">
@@ -1398,16 +1398,16 @@
         <v>8.170285701629298</v>
       </c>
       <c r="F31" t="n">
+        <v>46.88925756947324</v>
+      </c>
+      <c r="G31" t="n">
         <v>53.11074243052675</v>
       </c>
-      <c r="G31" t="n">
-        <v>46.88925756947324</v>
-      </c>
       <c r="H31" t="n">
+        <v>45.63316813639871</v>
+      </c>
+      <c r="I31" t="n">
         <v>54.36683186360129</v>
-      </c>
-      <c r="I31" t="n">
-        <v>45.63316813639871</v>
       </c>
     </row>
     <row r="32">
@@ -1429,16 +1429,16 @@
         <v>8.216111435100137</v>
       </c>
       <c r="F32" t="n">
+        <v>37.16042100034152</v>
+      </c>
+      <c r="G32" t="n">
         <v>62.83957899965849</v>
       </c>
-      <c r="G32" t="n">
-        <v>37.16042100034152</v>
-      </c>
       <c r="H32" t="n">
+        <v>47.14358392775758</v>
+      </c>
+      <c r="I32" t="n">
         <v>52.85641607224242</v>
-      </c>
-      <c r="I32" t="n">
-        <v>47.14358392775758</v>
       </c>
     </row>
     <row r="33">
@@ -1460,16 +1460,16 @@
         <v>8.173986994924645</v>
       </c>
       <c r="F33" t="n">
+        <v>54.20225957564067</v>
+      </c>
+      <c r="G33" t="n">
         <v>45.79774042435933</v>
       </c>
-      <c r="G33" t="n">
-        <v>54.20225957564067</v>
-      </c>
       <c r="H33" t="n">
+        <v>45.08917540009012</v>
+      </c>
+      <c r="I33" t="n">
         <v>54.91082459990988</v>
-      </c>
-      <c r="I33" t="n">
-        <v>45.08917540009012</v>
       </c>
     </row>
     <row r="34">
@@ -1491,16 +1491,16 @@
         <v>8.174392000139886</v>
       </c>
       <c r="F34" t="n">
+        <v>63.01194539249146</v>
+      </c>
+      <c r="G34" t="n">
         <v>36.98805460750853</v>
       </c>
-      <c r="G34" t="n">
-        <v>63.01194539249146</v>
-      </c>
       <c r="H34" t="n">
+        <v>44.81933266463522</v>
+      </c>
+      <c r="I34" t="n">
         <v>55.18066733536479</v>
-      </c>
-      <c r="I34" t="n">
-        <v>44.81933266463522</v>
       </c>
     </row>
     <row r="35">
@@ -1522,16 +1522,16 @@
         <v>8.165668500830414</v>
       </c>
       <c r="F35" t="n">
+        <v>23.34662777546282</v>
+      </c>
+      <c r="G35" t="n">
         <v>76.65337222453718</v>
       </c>
-      <c r="G35" t="n">
-        <v>23.34662777546282</v>
-      </c>
       <c r="H35" t="n">
+        <v>46.57106219780479</v>
+      </c>
+      <c r="I35" t="n">
         <v>53.42893780219522</v>
-      </c>
-      <c r="I35" t="n">
-        <v>46.57106219780479</v>
       </c>
     </row>
     <row r="36">
@@ -1553,16 +1553,16 @@
         <v>8.180847547304737</v>
       </c>
       <c r="F36" t="n">
+        <v>32.70421259248074</v>
+      </c>
+      <c r="G36" t="n">
         <v>67.29578740751924</v>
       </c>
-      <c r="G36" t="n">
-        <v>32.70421259248074</v>
-      </c>
       <c r="H36" t="n">
+        <v>46.29939921079762</v>
+      </c>
+      <c r="I36" t="n">
         <v>53.70060078920238</v>
-      </c>
-      <c r="I36" t="n">
-        <v>46.29939921079762</v>
       </c>
     </row>
     <row r="37">
@@ -1584,16 +1584,16 @@
         <v>8.170331378066015</v>
       </c>
       <c r="F37" t="n">
+        <v>37.14021000617665</v>
+      </c>
+      <c r="G37" t="n">
         <v>62.85978999382335</v>
       </c>
-      <c r="G37" t="n">
-        <v>37.14021000617665</v>
-      </c>
       <c r="H37" t="n">
+        <v>46.01314775482586</v>
+      </c>
+      <c r="I37" t="n">
         <v>53.98685224517414</v>
-      </c>
-      <c r="I37" t="n">
-        <v>46.01314775482586</v>
       </c>
     </row>
     <row r="38">
@@ -1615,16 +1615,16 @@
         <v>8.192124363163279</v>
       </c>
       <c r="F38" t="n">
+        <v>43.33181438444596</v>
+      </c>
+      <c r="G38" t="n">
         <v>56.66818561555404</v>
       </c>
-      <c r="G38" t="n">
-        <v>43.33181438444596</v>
-      </c>
       <c r="H38" t="n">
+        <v>45.83734475787041</v>
+      </c>
+      <c r="I38" t="n">
         <v>54.16265524212959</v>
-      </c>
-      <c r="I38" t="n">
-        <v>45.83734475787041</v>
       </c>
     </row>
     <row r="39">
@@ -1646,16 +1646,16 @@
         <v>8.180046203235266</v>
       </c>
       <c r="F39" t="n">
+        <v>47.22526587173703</v>
+      </c>
+      <c r="G39" t="n">
         <v>52.77473412826297</v>
       </c>
-      <c r="G39" t="n">
-        <v>47.22526587173703</v>
-      </c>
       <c r="H39" t="n">
+        <v>45.57188205967127</v>
+      </c>
+      <c r="I39" t="n">
         <v>54.42811794032873</v>
-      </c>
-      <c r="I39" t="n">
-        <v>45.57188205967127</v>
       </c>
     </row>
     <row r="40">
@@ -1677,16 +1677,16 @@
         <v>8.171404998224313</v>
       </c>
       <c r="F40" t="n">
+        <v>54.47197754331623</v>
+      </c>
+      <c r="G40" t="n">
         <v>45.52802245668377</v>
       </c>
-      <c r="G40" t="n">
-        <v>54.47197754331623</v>
-      </c>
       <c r="H40" t="n">
+        <v>45.25705683458704</v>
+      </c>
+      <c r="I40" t="n">
         <v>54.74294316541296</v>
-      </c>
-      <c r="I40" t="n">
-        <v>45.25705683458704</v>
       </c>
     </row>
     <row r="41">
@@ -1708,16 +1708,16 @@
         <v>8.196951724460543</v>
       </c>
       <c r="F41" t="n">
+        <v>45.15103838892385</v>
+      </c>
+      <c r="G41" t="n">
         <v>54.84896161107615</v>
       </c>
-      <c r="G41" t="n">
-        <v>45.15103838892385</v>
-      </c>
       <c r="H41" t="n">
+        <v>45.83576256804263</v>
+      </c>
+      <c r="I41" t="n">
         <v>54.16423743195737</v>
-      </c>
-      <c r="I41" t="n">
-        <v>45.83576256804263</v>
       </c>
     </row>
     <row r="42">
@@ -1739,16 +1739,16 @@
         <v>8.209829967840895</v>
       </c>
       <c r="F42" t="n">
+        <v>45.7182993497693</v>
+      </c>
+      <c r="G42" t="n">
         <v>54.2817006502307</v>
       </c>
-      <c r="G42" t="n">
-        <v>45.7182993497693</v>
-      </c>
       <c r="H42" t="n">
+        <v>45.6435820428943</v>
+      </c>
+      <c r="I42" t="n">
         <v>54.3564179571057</v>
-      </c>
-      <c r="I42" t="n">
-        <v>45.6435820428943</v>
       </c>
     </row>
     <row r="43">
@@ -1770,16 +1770,16 @@
         <v>8.18639659824442</v>
       </c>
       <c r="F43" t="n">
+        <v>17.88432523051132</v>
+      </c>
+      <c r="G43" t="n">
         <v>82.11567476948869</v>
       </c>
-      <c r="G43" t="n">
-        <v>17.88432523051132</v>
-      </c>
       <c r="H43" t="n">
+        <v>47.70078812783836</v>
+      </c>
+      <c r="I43" t="n">
         <v>52.29921187216164</v>
-      </c>
-      <c r="I43" t="n">
-        <v>47.70078812783836</v>
       </c>
     </row>
     <row r="44">
@@ -1801,16 +1801,16 @@
         <v>8.178534661468117</v>
       </c>
       <c r="F44" t="n">
+        <v>42.79512493166543</v>
+      </c>
+      <c r="G44" t="n">
         <v>57.20487506833457</v>
       </c>
-      <c r="G44" t="n">
-        <v>42.79512493166543</v>
-      </c>
       <c r="H44" t="n">
+        <v>46.16195142510932</v>
+      </c>
+      <c r="I44" t="n">
         <v>53.83804857489068</v>
-      </c>
-      <c r="I44" t="n">
-        <v>46.16195142510932</v>
       </c>
     </row>
     <row r="45">
@@ -1832,16 +1832,16 @@
         <v>8.176076214559371</v>
       </c>
       <c r="F45" t="n">
+        <v>49.28782770247024</v>
+      </c>
+      <c r="G45" t="n">
         <v>50.71217229752975</v>
       </c>
-      <c r="G45" t="n">
-        <v>49.28782770247024</v>
-      </c>
       <c r="H45" t="n">
+        <v>45.4345024082491</v>
+      </c>
+      <c r="I45" t="n">
         <v>54.5654975917509</v>
-      </c>
-      <c r="I45" t="n">
-        <v>45.4345024082491</v>
       </c>
     </row>
     <row r="46">
@@ -1863,16 +1863,16 @@
         <v>8.132823387582093</v>
       </c>
       <c r="F46" t="n">
+        <v>42.23256289629781</v>
+      </c>
+      <c r="G46" t="n">
         <v>57.76743710370219</v>
       </c>
-      <c r="G46" t="n">
-        <v>42.23256289629781</v>
-      </c>
       <c r="H46" t="n">
+        <v>46.2171078387873</v>
+      </c>
+      <c r="I46" t="n">
         <v>53.78289216121269</v>
-      </c>
-      <c r="I46" t="n">
-        <v>46.2171078387873</v>
       </c>
     </row>
     <row r="47">
@@ -1894,16 +1894,16 @@
         <v>8.141028447294214</v>
       </c>
       <c r="F47" t="n">
+        <v>39.22264095174758</v>
+      </c>
+      <c r="G47" t="n">
         <v>60.77735904825242</v>
       </c>
-      <c r="G47" t="n">
-        <v>39.22264095174758</v>
-      </c>
       <c r="H47" t="n">
+        <v>46.1099269918119</v>
+      </c>
+      <c r="I47" t="n">
         <v>53.8900730081881</v>
-      </c>
-      <c r="I47" t="n">
-        <v>46.1099269918119</v>
       </c>
     </row>
     <row r="48">
@@ -1925,16 +1925,16 @@
         <v>8.160158488235458</v>
       </c>
       <c r="F48" t="n">
+        <v>75.9312798843545</v>
+      </c>
+      <c r="G48" t="n">
         <v>24.0687201156455</v>
       </c>
-      <c r="G48" t="n">
-        <v>75.9312798843545</v>
-      </c>
       <c r="H48" t="n">
+        <v>44.4045697783063</v>
+      </c>
+      <c r="I48" t="n">
         <v>55.59543022169371</v>
-      </c>
-      <c r="I48" t="n">
-        <v>44.4045697783063</v>
       </c>
     </row>
     <row r="49">
@@ -1956,16 +1956,16 @@
         <v>8.148382411501569</v>
       </c>
       <c r="F49" t="n">
+        <v>46.48477380742827</v>
+      </c>
+      <c r="G49" t="n">
         <v>53.51522619257173</v>
       </c>
-      <c r="G49" t="n">
-        <v>46.48477380742827</v>
-      </c>
       <c r="H49" t="n">
+        <v>45.63325907273427</v>
+      </c>
+      <c r="I49" t="n">
         <v>54.36674092726573</v>
-      </c>
-      <c r="I49" t="n">
-        <v>45.63325907273427</v>
       </c>
     </row>
     <row r="50">
@@ -1987,16 +1987,16 @@
         <v>8.187779168923484</v>
       </c>
       <c r="F50" t="n">
+        <v>42.15987868284229</v>
+      </c>
+      <c r="G50" t="n">
         <v>57.84012131715771</v>
       </c>
-      <c r="G50" t="n">
-        <v>42.15987868284229</v>
-      </c>
       <c r="H50" t="n">
+        <v>46.09962239734718</v>
+      </c>
+      <c r="I50" t="n">
         <v>53.90037760265282</v>
-      </c>
-      <c r="I50" t="n">
-        <v>46.09962239734718</v>
       </c>
     </row>
     <row r="51">
@@ -2018,16 +2018,16 @@
         <v>8.196806558992048</v>
       </c>
       <c r="F51" t="n">
+        <v>40.62018088609178</v>
+      </c>
+      <c r="G51" t="n">
         <v>59.37981911390823</v>
       </c>
-      <c r="G51" t="n">
-        <v>40.62018088609178</v>
-      </c>
       <c r="H51" t="n">
+        <v>46.67432774074926</v>
+      </c>
+      <c r="I51" t="n">
         <v>53.32567225925074</v>
-      </c>
-      <c r="I51" t="n">
-        <v>46.67432774074926</v>
       </c>
     </row>
     <row r="52">
@@ -2049,16 +2049,16 @@
         <v>8.171401352776613</v>
       </c>
       <c r="F52" t="n">
+        <v>55.46170290421816</v>
+      </c>
+      <c r="G52" t="n">
         <v>44.53829709578184</v>
       </c>
-      <c r="G52" t="n">
-        <v>55.46170290421816</v>
-      </c>
       <c r="H52" t="n">
+        <v>45.24447809575639</v>
+      </c>
+      <c r="I52" t="n">
         <v>54.75552190424361</v>
-      </c>
-      <c r="I52" t="n">
-        <v>45.24447809575639</v>
       </c>
     </row>
     <row r="53">
@@ -2080,16 +2080,16 @@
         <v>8.195447522296892</v>
       </c>
       <c r="F53" t="n">
+        <v>57.12280701754386</v>
+      </c>
+      <c r="G53" t="n">
         <v>42.87719298245614</v>
       </c>
-      <c r="G53" t="n">
-        <v>57.12280701754386</v>
-      </c>
       <c r="H53" t="n">
+        <v>42.71363950098969</v>
+      </c>
+      <c r="I53" t="n">
         <v>57.2863604990103</v>
-      </c>
-      <c r="I53" t="n">
-        <v>42.71363950098969</v>
       </c>
     </row>
     <row r="54">
@@ -2111,16 +2111,16 @@
         <v>8.173059998623801</v>
       </c>
       <c r="F54" t="n">
+        <v>59.84523047862778</v>
+      </c>
+      <c r="G54" t="n">
         <v>40.15476952137221</v>
       </c>
-      <c r="G54" t="n">
-        <v>59.84523047862778</v>
-      </c>
       <c r="H54" t="n">
+        <v>44.55183610397295</v>
+      </c>
+      <c r="I54" t="n">
         <v>55.44816389602705</v>
-      </c>
-      <c r="I54" t="n">
-        <v>44.55183610397295</v>
       </c>
     </row>
     <row r="55">
@@ -2142,16 +2142,16 @@
         <v>8.187266173857896</v>
       </c>
       <c r="F55" t="n">
+        <v>38.54484786788825</v>
+      </c>
+      <c r="G55" t="n">
         <v>61.45515213211176</v>
       </c>
-      <c r="G55" t="n">
-        <v>38.54484786788825</v>
-      </c>
       <c r="H55" t="n">
+        <v>47.0494710121104</v>
+      </c>
+      <c r="I55" t="n">
         <v>52.9505289878896</v>
-      </c>
-      <c r="I55" t="n">
-        <v>47.0494710121104</v>
       </c>
     </row>
     <row r="56">
@@ -2173,16 +2173,16 @@
         <v>8.156506661621464</v>
       </c>
       <c r="F56" t="n">
+        <v>37.11621233859398</v>
+      </c>
+      <c r="G56" t="n">
         <v>62.88378766140602</v>
       </c>
-      <c r="G56" t="n">
-        <v>37.11621233859398</v>
-      </c>
       <c r="H56" t="n">
+        <v>46.11384068576208</v>
+      </c>
+      <c r="I56" t="n">
         <v>53.88615931423792</v>
-      </c>
-      <c r="I56" t="n">
-        <v>46.11384068576208</v>
       </c>
     </row>
     <row r="57">
@@ -2204,16 +2204,16 @@
         <v>8.17304064864102</v>
       </c>
       <c r="F57" t="n">
+        <v>54.63741371061445</v>
+      </c>
+      <c r="G57" t="n">
         <v>45.36258628938555</v>
       </c>
-      <c r="G57" t="n">
-        <v>54.63741371061445</v>
-      </c>
       <c r="H57" t="n">
+        <v>45.38148755919595</v>
+      </c>
+      <c r="I57" t="n">
         <v>54.61851244080405</v>
-      </c>
-      <c r="I57" t="n">
-        <v>45.38148755919595</v>
       </c>
     </row>
     <row r="58">
@@ -2235,16 +2235,16 @@
         <v>8.162490633522467</v>
       </c>
       <c r="F58" t="n">
+        <v>50.92772085294932</v>
+      </c>
+      <c r="G58" t="n">
         <v>49.07227914705068</v>
       </c>
-      <c r="G58" t="n">
-        <v>50.92772085294932</v>
-      </c>
       <c r="H58" t="n">
+        <v>45.37003915618541</v>
+      </c>
+      <c r="I58" t="n">
         <v>54.62996084381459</v>
-      </c>
-      <c r="I58" t="n">
-        <v>45.37003915618541</v>
       </c>
     </row>
     <row r="59">
@@ -2266,16 +2266,16 @@
         <v>8.156993414861066</v>
       </c>
       <c r="F59" t="n">
+        <v>54.20117776607459</v>
+      </c>
+      <c r="G59" t="n">
         <v>45.79882223392541</v>
       </c>
-      <c r="G59" t="n">
-        <v>54.20117776607459</v>
-      </c>
       <c r="H59" t="n">
+        <v>45.26556861403521</v>
+      </c>
+      <c r="I59" t="n">
         <v>54.73443138596479</v>
-      </c>
-      <c r="I59" t="n">
-        <v>45.26556861403521</v>
       </c>
     </row>
     <row r="60">
@@ -2297,16 +2297,16 @@
         <v>8.202796428058843</v>
       </c>
       <c r="F60" t="n">
+        <v>35.07970326257156</v>
+      </c>
+      <c r="G60" t="n">
         <v>64.92029673742846</v>
       </c>
-      <c r="G60" t="n">
-        <v>35.07970326257156</v>
-      </c>
       <c r="H60" t="n">
+        <v>46.71384635242779</v>
+      </c>
+      <c r="I60" t="n">
         <v>53.28615364757222</v>
-      </c>
-      <c r="I60" t="n">
-        <v>46.71384635242779</v>
       </c>
     </row>
     <row r="61">
@@ -2328,16 +2328,16 @@
         <v>8.175606177999839</v>
       </c>
       <c r="F61" t="n">
+        <v>60.49762951171402</v>
+      </c>
+      <c r="G61" t="n">
         <v>39.50237048828598</v>
       </c>
-      <c r="G61" t="n">
-        <v>60.49762951171402</v>
-      </c>
       <c r="H61" t="n">
+        <v>44.65158857591235</v>
+      </c>
+      <c r="I61" t="n">
         <v>55.34841142408765</v>
-      </c>
-      <c r="I61" t="n">
-        <v>44.65158857591235</v>
       </c>
     </row>
     <row r="62">
@@ -2359,16 +2359,16 @@
         <v>8.17272504544321</v>
       </c>
       <c r="F62" t="n">
+        <v>34.71197528620753</v>
+      </c>
+      <c r="G62" t="n">
         <v>65.28802471379248</v>
       </c>
-      <c r="G62" t="n">
-        <v>34.71197528620753</v>
-      </c>
       <c r="H62" t="n">
+        <v>46.41695973198101</v>
+      </c>
+      <c r="I62" t="n">
         <v>53.58304026801899</v>
-      </c>
-      <c r="I62" t="n">
-        <v>46.41695973198101</v>
       </c>
     </row>
     <row r="63">
@@ -2390,16 +2390,16 @@
         <v>8.168804828156295</v>
       </c>
       <c r="F63" t="n">
+        <v>27.25428795103551</v>
+      </c>
+      <c r="G63" t="n">
         <v>72.74571204896448</v>
       </c>
-      <c r="G63" t="n">
-        <v>27.25428795103551</v>
-      </c>
       <c r="H63" t="n">
+        <v>46.94014193448582</v>
+      </c>
+      <c r="I63" t="n">
         <v>53.05985806551418</v>
-      </c>
-      <c r="I63" t="n">
-        <v>46.94014193448582</v>
       </c>
     </row>
     <row r="64">
@@ -2421,16 +2421,16 @@
         <v>8.140287381531008</v>
       </c>
       <c r="F64" t="n">
+        <v>45.14368691008736</v>
+      </c>
+      <c r="G64" t="n">
         <v>54.85631308991265</v>
       </c>
-      <c r="G64" t="n">
-        <v>45.14368691008736</v>
-      </c>
       <c r="H64" t="n">
+        <v>45.74623481335047</v>
+      </c>
+      <c r="I64" t="n">
         <v>54.25376518664953</v>
-      </c>
-      <c r="I64" t="n">
-        <v>45.74623481335047</v>
       </c>
     </row>
     <row r="65">
@@ -2452,16 +2452,16 @@
         <v>8.164325826001601</v>
       </c>
       <c r="F65" t="n">
+        <v>24.42815385329189</v>
+      </c>
+      <c r="G65" t="n">
         <v>75.57184614670811</v>
       </c>
-      <c r="G65" t="n">
-        <v>24.42815385329189</v>
-      </c>
       <c r="H65" t="n">
+        <v>46.77831157304627</v>
+      </c>
+      <c r="I65" t="n">
         <v>53.22168842695373</v>
-      </c>
-      <c r="I65" t="n">
-        <v>46.77831157304627</v>
       </c>
     </row>
     <row r="66">
@@ -2483,16 +2483,16 @@
         <v>8.188571719496958</v>
       </c>
       <c r="F66" t="n">
+        <v>45.4656520524993</v>
+      </c>
+      <c r="G66" t="n">
         <v>54.53434794750069</v>
       </c>
-      <c r="G66" t="n">
-        <v>45.4656520524993</v>
-      </c>
       <c r="H66" t="n">
+        <v>45.70342186917607</v>
+      </c>
+      <c r="I66" t="n">
         <v>54.29657813082392</v>
-      </c>
-      <c r="I66" t="n">
-        <v>45.70342186917607</v>
       </c>
     </row>
     <row r="67">
@@ -2514,16 +2514,16 @@
         <v>8.217244726249033</v>
       </c>
       <c r="F67" t="n">
+        <v>42.46993662990869</v>
+      </c>
+      <c r="G67" t="n">
         <v>57.53006337009131</v>
       </c>
-      <c r="G67" t="n">
-        <v>42.46993662990869</v>
-      </c>
       <c r="H67" t="n">
+        <v>46.63196812730344</v>
+      </c>
+      <c r="I67" t="n">
         <v>53.36803187269656</v>
-      </c>
-      <c r="I67" t="n">
-        <v>46.63196812730344</v>
       </c>
     </row>
     <row r="68">
@@ -2545,16 +2545,16 @@
         <v>8.179244168965374</v>
       </c>
       <c r="F68" t="n">
+        <v>38.3241066935078</v>
+      </c>
+      <c r="G68" t="n">
         <v>61.6758933064922</v>
       </c>
-      <c r="G68" t="n">
-        <v>38.3241066935078</v>
-      </c>
       <c r="H68" t="n">
+        <v>45.96283791715776</v>
+      </c>
+      <c r="I68" t="n">
         <v>54.03716208284224</v>
-      </c>
-      <c r="I68" t="n">
-        <v>45.96283791715776</v>
       </c>
     </row>
     <row r="69">
@@ -2576,16 +2576,16 @@
         <v>8.161461048665165</v>
       </c>
       <c r="F69" t="n">
+        <v>42.29109736804257</v>
+      </c>
+      <c r="G69" t="n">
         <v>57.70890263195743</v>
       </c>
-      <c r="G69" t="n">
-        <v>42.29109736804257</v>
-      </c>
       <c r="H69" t="n">
+        <v>45.79839591687933</v>
+      </c>
+      <c r="I69" t="n">
         <v>54.20160408312067</v>
-      </c>
-      <c r="I69" t="n">
-        <v>45.79839591687933</v>
       </c>
     </row>
     <row r="70">
@@ -2607,16 +2607,16 @@
         <v>8.172324028962995</v>
       </c>
       <c r="F70" t="n">
+        <v>44.82532329666088</v>
+      </c>
+      <c r="G70" t="n">
         <v>55.17467670333912</v>
       </c>
-      <c r="G70" t="n">
-        <v>44.82532329666088</v>
-      </c>
       <c r="H70" t="n">
+        <v>45.80260715274715</v>
+      </c>
+      <c r="I70" t="n">
         <v>54.19739284725284</v>
-      </c>
-      <c r="I70" t="n">
-        <v>45.80260715274715</v>
       </c>
     </row>
     <row r="71">
@@ -2638,16 +2638,16 @@
         <v>8.183673811070022</v>
       </c>
       <c r="F71" t="n">
+        <v>38.41628122109158</v>
+      </c>
+      <c r="G71" t="n">
         <v>61.58371877890841</v>
       </c>
-      <c r="G71" t="n">
-        <v>38.41628122109158</v>
-      </c>
       <c r="H71" t="n">
+        <v>46.16178346098859</v>
+      </c>
+      <c r="I71" t="n">
         <v>53.8382165390114</v>
-      </c>
-      <c r="I71" t="n">
-        <v>46.16178346098859</v>
       </c>
     </row>
     <row r="72">
@@ -2669,16 +2669,16 @@
         <v>8.177600409320741</v>
       </c>
       <c r="F72" t="n">
+        <v>0.7254534083802376</v>
+      </c>
+      <c r="G72" t="n">
         <v>99.27454659161977</v>
       </c>
-      <c r="G72" t="n">
-        <v>0.7254534083802376</v>
-      </c>
       <c r="H72" t="n">
+        <v>47.37638085218306</v>
+      </c>
+      <c r="I72" t="n">
         <v>52.62361914781694</v>
-      </c>
-      <c r="I72" t="n">
-        <v>47.37638085218306</v>
       </c>
     </row>
     <row r="73">
@@ -2700,16 +2700,16 @@
         <v>8.15487603554401</v>
       </c>
       <c r="F73" t="n">
+        <v>53.35244558857946</v>
+      </c>
+      <c r="G73" t="n">
         <v>46.64755441142055</v>
       </c>
-      <c r="G73" t="n">
-        <v>53.35244558857946</v>
-      </c>
       <c r="H73" t="n">
+        <v>45.04526163432524</v>
+      </c>
+      <c r="I73" t="n">
         <v>54.95473836567475</v>
-      </c>
-      <c r="I73" t="n">
-        <v>45.04526163432524</v>
       </c>
     </row>
     <row r="74">
@@ -2731,16 +2731,16 @@
         <v>8.171402095307272</v>
       </c>
       <c r="F74" t="n">
+        <v>28.33957553058677</v>
+      </c>
+      <c r="G74" t="n">
         <v>71.66042446941323</v>
       </c>
-      <c r="G74" t="n">
-        <v>28.33957553058677</v>
-      </c>
       <c r="H74" t="n">
+        <v>46.58092706342652</v>
+      </c>
+      <c r="I74" t="n">
         <v>53.41907293657348</v>
-      </c>
-      <c r="I74" t="n">
-        <v>46.58092706342652</v>
       </c>
     </row>
     <row r="75">
@@ -2762,16 +2762,16 @@
         <v>8.172421952361521</v>
       </c>
       <c r="F75" t="n">
+        <v>35.39106328174456</v>
+      </c>
+      <c r="G75" t="n">
         <v>64.60893671825544</v>
       </c>
-      <c r="G75" t="n">
-        <v>35.39106328174456</v>
-      </c>
       <c r="H75" t="n">
+        <v>46.87919030916433</v>
+      </c>
+      <c r="I75" t="n">
         <v>53.12080969083568</v>
-      </c>
-      <c r="I75" t="n">
-        <v>46.87919030916433</v>
       </c>
     </row>
     <row r="76">
@@ -2793,16 +2793,16 @@
         <v>8.193800100957111</v>
       </c>
       <c r="F76" t="n">
+        <v>45.83874599463064</v>
+      </c>
+      <c r="G76" t="n">
         <v>54.16125400536936</v>
       </c>
-      <c r="G76" t="n">
-        <v>45.83874599463064</v>
-      </c>
       <c r="H76" t="n">
+        <v>45.67040588838954</v>
+      </c>
+      <c r="I76" t="n">
         <v>54.32959411161045</v>
-      </c>
-      <c r="I76" t="n">
-        <v>45.67040588838954</v>
       </c>
     </row>
     <row r="77">
@@ -2824,16 +2824,16 @@
         <v>8.16743789212512</v>
       </c>
       <c r="F77" t="n">
+        <v>27.28878196104528</v>
+      </c>
+      <c r="G77" t="n">
         <v>72.71121803895473</v>
       </c>
-      <c r="G77" t="n">
-        <v>27.28878196104528</v>
-      </c>
       <c r="H77" t="n">
+        <v>47.47295421646062</v>
+      </c>
+      <c r="I77" t="n">
         <v>52.52704578353939</v>
-      </c>
-      <c r="I77" t="n">
-        <v>47.47295421646062</v>
       </c>
     </row>
     <row r="78">
@@ -2855,16 +2855,16 @@
         <v>8.276897969050479</v>
       </c>
       <c r="F78" t="n">
+        <v>43.51014682787748</v>
+      </c>
+      <c r="G78" t="n">
         <v>56.48985317212253</v>
       </c>
-      <c r="G78" t="n">
-        <v>43.51014682787748</v>
-      </c>
       <c r="H78" t="n">
+        <v>46.06766659490148</v>
+      </c>
+      <c r="I78" t="n">
         <v>53.93233340509852</v>
-      </c>
-      <c r="I78" t="n">
-        <v>46.06766659490148</v>
       </c>
     </row>
     <row r="79">
@@ -2886,16 +2886,16 @@
         <v>8.168384574121886</v>
       </c>
       <c r="F79" t="n">
+        <v>50.84210105212625</v>
+      </c>
+      <c r="G79" t="n">
         <v>49.15789894787375</v>
       </c>
-      <c r="G79" t="n">
-        <v>50.84210105212625</v>
-      </c>
       <c r="H79" t="n">
+        <v>45.37890729024968</v>
+      </c>
+      <c r="I79" t="n">
         <v>54.62109270975032</v>
-      </c>
-      <c r="I79" t="n">
-        <v>45.37890729024968</v>
       </c>
     </row>
     <row r="80">
@@ -2917,16 +2917,16 @@
         <v>8.133220232674564</v>
       </c>
       <c r="F80" t="n">
+        <v>42.57078047551038</v>
+      </c>
+      <c r="G80" t="n">
         <v>57.42921952448962</v>
       </c>
-      <c r="G80" t="n">
-        <v>42.57078047551038</v>
-      </c>
       <c r="H80" t="n">
+        <v>46.17328321549363</v>
+      </c>
+      <c r="I80" t="n">
         <v>53.82671678450637</v>
-      </c>
-      <c r="I80" t="n">
-        <v>46.17328321549363</v>
       </c>
     </row>
     <row r="81">
@@ -2948,16 +2948,16 @@
         <v>8.151489847438832</v>
       </c>
       <c r="F81" t="n">
+        <v>52.84680315764526</v>
+      </c>
+      <c r="G81" t="n">
         <v>47.15319684235475</v>
       </c>
-      <c r="G81" t="n">
-        <v>52.84680315764526</v>
-      </c>
       <c r="H81" t="n">
+        <v>43.32333670568965</v>
+      </c>
+      <c r="I81" t="n">
         <v>56.67666329431034</v>
-      </c>
-      <c r="I81" t="n">
-        <v>43.32333670568965</v>
       </c>
     </row>
     <row r="82">
@@ -2979,16 +2979,16 @@
         <v>8.159143167688468</v>
       </c>
       <c r="F82" t="n">
+        <v>71.03891015401308</v>
+      </c>
+      <c r="G82" t="n">
         <v>28.96108984598692</v>
       </c>
-      <c r="G82" t="n">
-        <v>71.03891015401308</v>
-      </c>
       <c r="H82" t="n">
+        <v>43.62964503774762</v>
+      </c>
+      <c r="I82" t="n">
         <v>56.37035496225238</v>
-      </c>
-      <c r="I82" t="n">
-        <v>43.62964503774762</v>
       </c>
     </row>
     <row r="83">
@@ -3010,16 +3010,16 @@
         <v>8.171359688230545</v>
       </c>
       <c r="F83" t="n">
+        <v>49.02269755590572</v>
+      </c>
+      <c r="G83" t="n">
         <v>50.97730244409428</v>
       </c>
-      <c r="G83" t="n">
-        <v>49.02269755590572</v>
-      </c>
       <c r="H83" t="n">
+        <v>45.44657962508526</v>
+      </c>
+      <c r="I83" t="n">
         <v>54.55342037491474</v>
-      </c>
-      <c r="I83" t="n">
-        <v>45.44657962508526</v>
       </c>
     </row>
     <row r="84">
@@ -3041,16 +3041,16 @@
         <v>8.189139944844021</v>
       </c>
       <c r="F84" t="n">
+        <v>44.20495566536992</v>
+      </c>
+      <c r="G84" t="n">
         <v>55.79504433463007</v>
       </c>
-      <c r="G84" t="n">
-        <v>44.20495566536992</v>
-      </c>
       <c r="H84" t="n">
+        <v>45.79039442897205</v>
+      </c>
+      <c r="I84" t="n">
         <v>54.20960557102794</v>
-      </c>
-      <c r="I84" t="n">
-        <v>45.79039442897205</v>
       </c>
     </row>
     <row r="85">
@@ -3072,16 +3072,16 @@
         <v>8.170416707328743</v>
       </c>
       <c r="F85" t="n">
+        <v>30.99255697841061</v>
+      </c>
+      <c r="G85" t="n">
         <v>69.00744302158938</v>
       </c>
-      <c r="G85" t="n">
-        <v>30.99255697841061</v>
-      </c>
       <c r="H85" t="n">
+        <v>46.44452536156865</v>
+      </c>
+      <c r="I85" t="n">
         <v>53.55547463843136</v>
-      </c>
-      <c r="I85" t="n">
-        <v>46.44452536156865</v>
       </c>
     </row>
     <row r="86">
@@ -3103,16 +3103,16 @@
         <v>8.176680776723458</v>
       </c>
       <c r="F86" t="n">
+        <v>53.8217776420281</v>
+      </c>
+      <c r="G86" t="n">
         <v>46.1782223579719</v>
       </c>
-      <c r="G86" t="n">
-        <v>53.8217776420281</v>
-      </c>
       <c r="H86" t="n">
+        <v>45.17542382260804</v>
+      </c>
+      <c r="I86" t="n">
         <v>54.82457617739196</v>
-      </c>
-      <c r="I86" t="n">
-        <v>45.17542382260804</v>
       </c>
     </row>
     <row r="87">
@@ -3134,16 +3134,16 @@
         <v>8.163653316232191</v>
       </c>
       <c r="F87" t="n">
+        <v>38.90803714517793</v>
+      </c>
+      <c r="G87" t="n">
         <v>61.09196285482207</v>
       </c>
-      <c r="G87" t="n">
-        <v>38.90803714517793</v>
-      </c>
       <c r="H87" t="n">
+        <v>46.46737141746769</v>
+      </c>
+      <c r="I87" t="n">
         <v>53.5326285825323</v>
-      </c>
-      <c r="I87" t="n">
-        <v>46.46737141746769</v>
       </c>
     </row>
     <row r="88">
@@ -3165,16 +3165,16 @@
         <v>8.187680612763026</v>
       </c>
       <c r="F88" t="n">
+        <v>58.1116147680988</v>
+      </c>
+      <c r="G88" t="n">
         <v>41.8883852319012</v>
       </c>
-      <c r="G88" t="n">
-        <v>58.1116147680988</v>
-      </c>
       <c r="H88" t="n">
+        <v>43.7021888765797</v>
+      </c>
+      <c r="I88" t="n">
         <v>56.2978111234203</v>
-      </c>
-      <c r="I88" t="n">
-        <v>43.7021888765797</v>
       </c>
     </row>
     <row r="89">
@@ -3196,16 +3196,16 @@
         <v>8.165218091609944</v>
       </c>
       <c r="F89" t="n">
+        <v>92.53872120730739</v>
+      </c>
+      <c r="G89" t="n">
         <v>7.461278792692613</v>
       </c>
-      <c r="G89" t="n">
-        <v>92.53872120730739</v>
-      </c>
       <c r="H89" t="n">
+        <v>43.44985415135058</v>
+      </c>
+      <c r="I89" t="n">
         <v>56.55014584864941</v>
-      </c>
-      <c r="I89" t="n">
-        <v>43.44985415135058</v>
       </c>
     </row>
     <row r="90">
@@ -3227,16 +3227,16 @@
         <v>8.179038512406164</v>
       </c>
       <c r="F90" t="n">
+        <v>48.85726606295817</v>
+      </c>
+      <c r="G90" t="n">
         <v>51.14273393704183</v>
       </c>
-      <c r="G90" t="n">
-        <v>48.85726606295817</v>
-      </c>
       <c r="H90" t="n">
+        <v>45.41715700846868</v>
+      </c>
+      <c r="I90" t="n">
         <v>54.58284299153131</v>
-      </c>
-      <c r="I90" t="n">
-        <v>45.41715700846868</v>
       </c>
     </row>
     <row r="91">
@@ -3258,16 +3258,16 @@
         <v>8.16013722150811</v>
       </c>
       <c r="F91" t="n">
+        <v>35.04367357125031</v>
+      </c>
+      <c r="G91" t="n">
         <v>64.95632642874969</v>
       </c>
-      <c r="G91" t="n">
-        <v>35.04367357125031</v>
-      </c>
       <c r="H91" t="n">
+        <v>46.19362272659379</v>
+      </c>
+      <c r="I91" t="n">
         <v>53.80637727340621</v>
-      </c>
-      <c r="I91" t="n">
-        <v>46.19362272659379</v>
       </c>
     </row>
     <row r="92">
@@ -3289,16 +3289,16 @@
         <v>8.18548124572939</v>
       </c>
       <c r="F92" t="n">
+        <v>17.55235788573871</v>
+      </c>
+      <c r="G92" t="n">
         <v>82.44764211426128</v>
       </c>
-      <c r="G92" t="n">
-        <v>17.55235788573871</v>
-      </c>
       <c r="H92" t="n">
+        <v>47.5972717033485</v>
+      </c>
+      <c r="I92" t="n">
         <v>52.4027282966515</v>
-      </c>
-      <c r="I92" t="n">
-        <v>47.5972717033485</v>
       </c>
     </row>
     <row r="93">
@@ -3320,16 +3320,16 @@
         <v>8.166380776850358</v>
       </c>
       <c r="F93" t="n">
+        <v>40.43511902052706</v>
+      </c>
+      <c r="G93" t="n">
         <v>59.56488097947295</v>
       </c>
-      <c r="G93" t="n">
-        <v>40.43511902052706</v>
-      </c>
       <c r="H93" t="n">
+        <v>45.96289565385156</v>
+      </c>
+      <c r="I93" t="n">
         <v>54.03710434614845</v>
-      </c>
-      <c r="I93" t="n">
-        <v>45.96289565385156</v>
       </c>
     </row>
     <row r="94">
@@ -3351,16 +3351,16 @@
         <v>8.171685977678935</v>
       </c>
       <c r="F94" t="n">
+        <v>37.29719626168225</v>
+      </c>
+      <c r="G94" t="n">
         <v>62.70280373831775</v>
       </c>
-      <c r="G94" t="n">
-        <v>37.29719626168225</v>
-      </c>
       <c r="H94" t="n">
+        <v>47.55036452744189</v>
+      </c>
+      <c r="I94" t="n">
         <v>52.44963547255811</v>
-      </c>
-      <c r="I94" t="n">
-        <v>47.55036452744189</v>
       </c>
     </row>
     <row r="95">
@@ -3382,16 +3382,16 @@
         <v>8.184641486336929</v>
       </c>
       <c r="F95" t="n">
+        <v>54.0962494351559</v>
+      </c>
+      <c r="G95" t="n">
         <v>45.9037505648441</v>
       </c>
-      <c r="G95" t="n">
-        <v>54.0962494351559</v>
-      </c>
       <c r="H95" t="n">
+        <v>44.75190791691192</v>
+      </c>
+      <c r="I95" t="n">
         <v>55.24809208308808</v>
-      </c>
-      <c r="I95" t="n">
-        <v>44.75190791691192</v>
       </c>
     </row>
     <row r="96">
@@ -3413,16 +3413,16 @@
         <v>8.179967926480547</v>
       </c>
       <c r="F96" t="n">
+        <v>44.19029864123615</v>
+      </c>
+      <c r="G96" t="n">
         <v>55.80970135876385</v>
       </c>
-      <c r="G96" t="n">
-        <v>44.19029864123615</v>
-      </c>
       <c r="H96" t="n">
+        <v>45.78893073799107</v>
+      </c>
+      <c r="I96" t="n">
         <v>54.21106926200893</v>
-      </c>
-      <c r="I96" t="n">
-        <v>45.78893073799107</v>
       </c>
     </row>
     <row r="97">
@@ -3444,16 +3444,16 @@
         <v>8.179584220507278</v>
       </c>
       <c r="F97" t="n">
+        <v>40.04071531215072</v>
+      </c>
+      <c r="G97" t="n">
         <v>59.95928468784927</v>
       </c>
-      <c r="G97" t="n">
-        <v>40.04071531215072</v>
-      </c>
       <c r="H97" t="n">
+        <v>46.02746891511222</v>
+      </c>
+      <c r="I97" t="n">
         <v>53.97253108488778</v>
-      </c>
-      <c r="I97" t="n">
-        <v>46.02746891511222</v>
       </c>
     </row>
     <row r="98">
@@ -3475,16 +3475,16 @@
         <v>8.138679922596918</v>
       </c>
       <c r="F98" t="n">
+        <v>43.71610383975703</v>
+      </c>
+      <c r="G98" t="n">
         <v>56.28389616024296</v>
       </c>
-      <c r="G98" t="n">
-        <v>43.71610383975703</v>
-      </c>
       <c r="H98" t="n">
+        <v>45.81969113087822</v>
+      </c>
+      <c r="I98" t="n">
         <v>54.18030886912179</v>
-      </c>
-      <c r="I98" t="n">
-        <v>45.81969113087822</v>
       </c>
     </row>
     <row r="99">
@@ -3506,16 +3506,16 @@
         <v>8.160648645033273</v>
       </c>
       <c r="F99" t="n">
+        <v>64.60316862981222</v>
+      </c>
+      <c r="G99" t="n">
         <v>35.39683137018778</v>
       </c>
-      <c r="G99" t="n">
-        <v>64.60316862981222</v>
-      </c>
       <c r="H99" t="n">
+        <v>44.47754436580203</v>
+      </c>
+      <c r="I99" t="n">
         <v>55.52245563419797</v>
-      </c>
-      <c r="I99" t="n">
-        <v>44.47754436580203</v>
       </c>
     </row>
     <row r="100">
@@ -3537,16 +3537,16 @@
         <v>8.173545741361297</v>
       </c>
       <c r="F100" t="n">
+        <v>36.91557608416731</v>
+      </c>
+      <c r="G100" t="n">
         <v>63.08442391583269</v>
       </c>
-      <c r="G100" t="n">
-        <v>36.91557608416731</v>
-      </c>
       <c r="H100" t="n">
+        <v>46.09273812596341</v>
+      </c>
+      <c r="I100" t="n">
         <v>53.90726187403659</v>
-      </c>
-      <c r="I100" t="n">
-        <v>46.09273812596341</v>
       </c>
     </row>
     <row r="101">
@@ -3568,16 +3568,16 @@
         <v>8.16027438230318</v>
       </c>
       <c r="F101" t="n">
+        <v>51.40384353277907</v>
+      </c>
+      <c r="G101" t="n">
         <v>48.59615646722094</v>
       </c>
-      <c r="G101" t="n">
-        <v>51.40384353277907</v>
-      </c>
       <c r="H101" t="n">
+        <v>45.49164208456244</v>
+      </c>
+      <c r="I101" t="n">
         <v>54.50835791543756</v>
-      </c>
-      <c r="I101" t="n">
-        <v>45.49164208456244</v>
       </c>
     </row>
     <row r="102">
@@ -3599,16 +3599,16 @@
         <v>8.178774558662738</v>
       </c>
       <c r="F102" t="n">
+        <v>53.53813164273728</v>
+      </c>
+      <c r="G102" t="n">
         <v>46.46186835726272</v>
       </c>
-      <c r="G102" t="n">
-        <v>53.53813164273728</v>
-      </c>
       <c r="H102" t="n">
+        <v>45.28739514989461</v>
+      </c>
+      <c r="I102" t="n">
         <v>54.71260485010539</v>
-      </c>
-      <c r="I102" t="n">
-        <v>45.28739514989461</v>
       </c>
     </row>
     <row r="103">
@@ -3630,16 +3630,16 @@
         <v>8.15150346547736</v>
       </c>
       <c r="F103" t="n">
+        <v>41.22551977618081</v>
+      </c>
+      <c r="G103" t="n">
         <v>58.77448022381919</v>
       </c>
-      <c r="G103" t="n">
-        <v>41.22551977618081</v>
-      </c>
       <c r="H103" t="n">
+        <v>45.88004768818537</v>
+      </c>
+      <c r="I103" t="n">
         <v>54.11995231181464</v>
-      </c>
-      <c r="I103" t="n">
-        <v>45.88004768818537</v>
       </c>
     </row>
     <row r="104">
@@ -3661,16 +3661,16 @@
         <v>8.15817390591233</v>
       </c>
       <c r="F104" t="n">
+        <v>39.2086688537628</v>
+      </c>
+      <c r="G104" t="n">
         <v>60.79133114623721</v>
       </c>
-      <c r="G104" t="n">
-        <v>39.2086688537628</v>
-      </c>
       <c r="H104" t="n">
+        <v>45.99711640613143</v>
+      </c>
+      <c r="I104" t="n">
         <v>54.00288359386857</v>
-      </c>
-      <c r="I104" t="n">
-        <v>45.99711640613143</v>
       </c>
     </row>
     <row r="105">
@@ -3692,16 +3692,16 @@
         <v>8.133275300310123</v>
       </c>
       <c r="F105" t="n">
+        <v>42.28363929796248</v>
+      </c>
+      <c r="G105" t="n">
         <v>57.71636070203753</v>
       </c>
-      <c r="G105" t="n">
-        <v>42.28363929796248</v>
-      </c>
       <c r="H105" t="n">
+        <v>46.21766536761437</v>
+      </c>
+      <c r="I105" t="n">
         <v>53.78233463238563</v>
-      </c>
-      <c r="I105" t="n">
-        <v>46.21766536761437</v>
       </c>
     </row>
     <row r="106">
@@ -3723,16 +3723,16 @@
         <v>8.174204357480399</v>
       </c>
       <c r="F106" t="n">
+        <v>48.76080484918045</v>
+      </c>
+      <c r="G106" t="n">
         <v>51.23919515081955</v>
       </c>
-      <c r="G106" t="n">
-        <v>48.76080484918045</v>
-      </c>
       <c r="H106" t="n">
+        <v>45.48103195444673</v>
+      </c>
+      <c r="I106" t="n">
         <v>54.51896804555327</v>
-      </c>
-      <c r="I106" t="n">
-        <v>45.48103195444673</v>
       </c>
     </row>
     <row r="107">
@@ -3754,16 +3754,16 @@
         <v>8.165463130836123</v>
       </c>
       <c r="F107" t="n">
+        <v>46.42272794883237</v>
+      </c>
+      <c r="G107" t="n">
         <v>53.57727205116763</v>
       </c>
-      <c r="G107" t="n">
-        <v>46.42272794883237</v>
-      </c>
       <c r="H107" t="n">
+        <v>45.65285963310367</v>
+      </c>
+      <c r="I107" t="n">
         <v>54.34714036689632</v>
-      </c>
-      <c r="I107" t="n">
-        <v>45.65285963310367</v>
       </c>
     </row>
     <row r="108">
@@ -3785,16 +3785,16 @@
         <v>8.164050158545852</v>
       </c>
       <c r="F108" t="n">
+        <v>36.01521498387019</v>
+      </c>
+      <c r="G108" t="n">
         <v>63.98478501612981</v>
       </c>
-      <c r="G108" t="n">
-        <v>36.01521498387019</v>
-      </c>
       <c r="H108" t="n">
+        <v>46.16513674310347</v>
+      </c>
+      <c r="I108" t="n">
         <v>53.83486325689653</v>
-      </c>
-      <c r="I108" t="n">
-        <v>46.16513674310347</v>
       </c>
     </row>
     <row r="109">
@@ -3816,16 +3816,16 @@
         <v>8.157911071243042</v>
       </c>
       <c r="F109" t="n">
+        <v>44.47897843633297</v>
+      </c>
+      <c r="G109" t="n">
         <v>55.52102156366703</v>
       </c>
-      <c r="G109" t="n">
-        <v>44.47897843633297</v>
-      </c>
       <c r="H109" t="n">
+        <v>45.81335918003342</v>
+      </c>
+      <c r="I109" t="n">
         <v>54.18664081996658</v>
-      </c>
-      <c r="I109" t="n">
-        <v>45.81335918003342</v>
       </c>
     </row>
     <row r="110">
@@ -3847,16 +3847,16 @@
         <v>8.146363746005381</v>
       </c>
       <c r="F110" t="n">
+        <v>65.60308392550276</v>
+      </c>
+      <c r="G110" t="n">
         <v>34.39691607449723</v>
       </c>
-      <c r="G110" t="n">
-        <v>65.60308392550276</v>
-      </c>
       <c r="H110" t="n">
+        <v>44.6677595810442</v>
+      </c>
+      <c r="I110" t="n">
         <v>55.33224041895581</v>
-      </c>
-      <c r="I110" t="n">
-        <v>44.6677595810442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tables and checked for replication with AofUresults
</commit_message>
<xml_diff>
--- a/tables_plots/phenotype_statistics.xlsx
+++ b/tables_plots/phenotype_statistics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,16 @@
           <t>%Men_Controls</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Cases</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Controls</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -510,6 +520,12 @@
       <c r="I2" t="n">
         <v>53.77032281991568</v>
       </c>
+      <c r="J2" t="n">
+        <v>75108</v>
+      </c>
+      <c r="K2" t="n">
+        <v>366706</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,6 +557,12 @@
       <c r="I3" t="n">
         <v>56.0331485935376</v>
       </c>
+      <c r="J3" t="n">
+        <v>59294</v>
+      </c>
+      <c r="K3" t="n">
+        <v>382520</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -572,6 +594,12 @@
       <c r="I4" t="n">
         <v>54.12429433975225</v>
       </c>
+      <c r="J4" t="n">
+        <v>34217</v>
+      </c>
+      <c r="K4" t="n">
+        <v>407597</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -603,6 +631,12 @@
       <c r="I5" t="n">
         <v>56.53199844444899</v>
       </c>
+      <c r="J5" t="n">
+        <v>99813</v>
+      </c>
+      <c r="K5" t="n">
+        <v>342001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -634,6 +668,12 @@
       <c r="I6" t="n">
         <v>55.60404442829024</v>
       </c>
+      <c r="J6" t="n">
+        <v>18120</v>
+      </c>
+      <c r="K6" t="n">
+        <v>423694</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -665,6 +705,12 @@
       <c r="I7" t="n">
         <v>54.3735112196489</v>
       </c>
+      <c r="J7" t="n">
+        <v>42158</v>
+      </c>
+      <c r="K7" t="n">
+        <v>399656</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -696,6 +742,12 @@
       <c r="I8" t="n">
         <v>50.72457045764144</v>
       </c>
+      <c r="J8" t="n">
+        <v>32192</v>
+      </c>
+      <c r="K8" t="n">
+        <v>409622</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -727,6 +779,12 @@
       <c r="I9" t="n">
         <v>53.63155590785939</v>
       </c>
+      <c r="J9" t="n">
+        <v>19199</v>
+      </c>
+      <c r="K9" t="n">
+        <v>422615</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -758,6 +816,12 @@
       <c r="I10" t="n">
         <v>54.04350681006436</v>
       </c>
+      <c r="J10" t="n">
+        <v>39762</v>
+      </c>
+      <c r="K10" t="n">
+        <v>402052</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -789,6 +853,12 @@
       <c r="I11" t="n">
         <v>53.99262768382849</v>
       </c>
+      <c r="J11" t="n">
+        <v>19423</v>
+      </c>
+      <c r="K11" t="n">
+        <v>422391</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -820,6 +890,12 @@
       <c r="I12" t="n">
         <v>51.46076061994253</v>
       </c>
+      <c r="J12" t="n">
+        <v>25969</v>
+      </c>
+      <c r="K12" t="n">
+        <v>415845</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -851,6 +927,12 @@
       <c r="I13" t="n">
         <v>54.26503063068622</v>
       </c>
+      <c r="J13" t="n">
+        <v>52825</v>
+      </c>
+      <c r="K13" t="n">
+        <v>388989</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -882,6 +964,12 @@
       <c r="I14" t="n">
         <v>53.98761638952084</v>
       </c>
+      <c r="J14" t="n">
+        <v>15444</v>
+      </c>
+      <c r="K14" t="n">
+        <v>426370</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -913,6 +1001,12 @@
       <c r="I15" t="n">
         <v>53.32596039679805</v>
       </c>
+      <c r="J15" t="n">
+        <v>24070</v>
+      </c>
+      <c r="K15" t="n">
+        <v>417744</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -944,6 +1038,12 @@
       <c r="I16" t="n">
         <v>54.27379029715743</v>
       </c>
+      <c r="J16" t="n">
+        <v>29440</v>
+      </c>
+      <c r="K16" t="n">
+        <v>412374</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -975,6 +1075,12 @@
       <c r="I17" t="n">
         <v>57.25312692375603</v>
       </c>
+      <c r="J17" t="n">
+        <v>22712</v>
+      </c>
+      <c r="K17" t="n">
+        <v>419102</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1006,6 +1112,12 @@
       <c r="I18" t="n">
         <v>57.80520415509617</v>
       </c>
+      <c r="J18" t="n">
+        <v>150124</v>
+      </c>
+      <c r="K18" t="n">
+        <v>291690</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1037,6 +1149,12 @@
       <c r="I19" t="n">
         <v>53.66694834813936</v>
       </c>
+      <c r="J19" t="n">
+        <v>19351</v>
+      </c>
+      <c r="K19" t="n">
+        <v>422463</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1068,6 +1186,12 @@
       <c r="I20" t="n">
         <v>54.57071415443843</v>
       </c>
+      <c r="J20" t="n">
+        <v>28290</v>
+      </c>
+      <c r="K20" t="n">
+        <v>413524</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1099,6 +1223,12 @@
       <c r="I21" t="n">
         <v>54.3559325838773</v>
       </c>
+      <c r="J21" t="n">
+        <v>40901</v>
+      </c>
+      <c r="K21" t="n">
+        <v>400913</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1130,6 +1260,12 @@
       <c r="I22" t="n">
         <v>53.78304751911978</v>
       </c>
+      <c r="J22" t="n">
+        <v>26276</v>
+      </c>
+      <c r="K22" t="n">
+        <v>415538</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1161,6 +1297,12 @@
       <c r="I23" t="n">
         <v>54.23444924995314</v>
       </c>
+      <c r="J23" t="n">
+        <v>20307</v>
+      </c>
+      <c r="K23" t="n">
+        <v>421507</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1192,6 +1334,12 @@
       <c r="I24" t="n">
         <v>53.15501364980126</v>
       </c>
+      <c r="J24" t="n">
+        <v>17632</v>
+      </c>
+      <c r="K24" t="n">
+        <v>424182</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1223,6 +1371,12 @@
       <c r="I25" t="n">
         <v>53.25162378326507</v>
       </c>
+      <c r="J25" t="n">
+        <v>158371</v>
+      </c>
+      <c r="K25" t="n">
+        <v>283443</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1254,6 +1408,12 @@
       <c r="I26" t="n">
         <v>54.12532727877942</v>
       </c>
+      <c r="J26" t="n">
+        <v>39252</v>
+      </c>
+      <c r="K26" t="n">
+        <v>402562</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1285,6 +1445,12 @@
       <c r="I27" t="n">
         <v>54.73901489987662</v>
       </c>
+      <c r="J27" t="n">
+        <v>20334</v>
+      </c>
+      <c r="K27" t="n">
+        <v>421480</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1316,6 +1482,12 @@
       <c r="I28" t="n">
         <v>54.76646972911571</v>
       </c>
+      <c r="J28" t="n">
+        <v>109052</v>
+      </c>
+      <c r="K28" t="n">
+        <v>332762</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1347,6 +1519,12 @@
       <c r="I29" t="n">
         <v>56.92749976680722</v>
       </c>
+      <c r="J29" t="n">
+        <v>23705</v>
+      </c>
+      <c r="K29" t="n">
+        <v>418109</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1378,6 +1556,12 @@
       <c r="I30" t="n">
         <v>55.54253867700303</v>
       </c>
+      <c r="J30" t="n">
+        <v>26968</v>
+      </c>
+      <c r="K30" t="n">
+        <v>414846</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1409,6 +1593,12 @@
       <c r="I31" t="n">
         <v>54.36683186360129</v>
       </c>
+      <c r="J31" t="n">
+        <v>19288</v>
+      </c>
+      <c r="K31" t="n">
+        <v>422526</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1440,6 +1630,12 @@
       <c r="I32" t="n">
         <v>52.85641607224242</v>
       </c>
+      <c r="J32" t="n">
+        <v>64418</v>
+      </c>
+      <c r="K32" t="n">
+        <v>377396</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1471,6 +1667,12 @@
       <c r="I33" t="n">
         <v>54.91082459990988</v>
       </c>
+      <c r="J33" t="n">
+        <v>29032</v>
+      </c>
+      <c r="K33" t="n">
+        <v>412782</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1502,6 +1704,12 @@
       <c r="I34" t="n">
         <v>55.18066733536479</v>
       </c>
+      <c r="J34" t="n">
+        <v>21096</v>
+      </c>
+      <c r="K34" t="n">
+        <v>420718</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1533,6 +1741,12 @@
       <c r="I35" t="n">
         <v>53.42893780219522</v>
       </c>
+      <c r="J35" t="n">
+        <v>16799</v>
+      </c>
+      <c r="K35" t="n">
+        <v>425015</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1564,6 +1778,12 @@
       <c r="I36" t="n">
         <v>53.70060078920238</v>
       </c>
+      <c r="J36" t="n">
+        <v>19869</v>
+      </c>
+      <c r="K36" t="n">
+        <v>421945</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1595,6 +1815,12 @@
       <c r="I37" t="n">
         <v>53.98685224517414</v>
       </c>
+      <c r="J37" t="n">
+        <v>16190</v>
+      </c>
+      <c r="K37" t="n">
+        <v>425624</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1626,6 +1852,12 @@
       <c r="I38" t="n">
         <v>54.16265524212959</v>
       </c>
+      <c r="J38" t="n">
+        <v>26334</v>
+      </c>
+      <c r="K38" t="n">
+        <v>415480</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1657,6 +1889,12 @@
       <c r="I39" t="n">
         <v>54.42811794032873</v>
       </c>
+      <c r="J39" t="n">
+        <v>31030</v>
+      </c>
+      <c r="K39" t="n">
+        <v>410784</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1688,6 +1926,12 @@
       <c r="I40" t="n">
         <v>54.74294316541296</v>
       </c>
+      <c r="J40" t="n">
+        <v>20662</v>
+      </c>
+      <c r="K40" t="n">
+        <v>421152</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1719,6 +1963,12 @@
       <c r="I41" t="n">
         <v>54.16423743195737</v>
       </c>
+      <c r="J41" t="n">
+        <v>95340</v>
+      </c>
+      <c r="K41" t="n">
+        <v>346474</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1750,6 +2000,12 @@
       <c r="I42" t="n">
         <v>54.3564179571057</v>
       </c>
+      <c r="J42" t="n">
+        <v>262676</v>
+      </c>
+      <c r="K42" t="n">
+        <v>179138</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1781,6 +2037,12 @@
       <c r="I43" t="n">
         <v>52.29921187216164</v>
       </c>
+      <c r="J43" t="n">
+        <v>29825</v>
+      </c>
+      <c r="K43" t="n">
+        <v>411989</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1812,6 +2074,12 @@
       <c r="I44" t="n">
         <v>53.83804857489068</v>
       </c>
+      <c r="J44" t="n">
+        <v>62194</v>
+      </c>
+      <c r="K44" t="n">
+        <v>379620</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1843,6 +2111,12 @@
       <c r="I45" t="n">
         <v>54.5654975917509</v>
       </c>
+      <c r="J45" t="n">
+        <v>29066</v>
+      </c>
+      <c r="K45" t="n">
+        <v>412748</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1874,6 +2148,12 @@
       <c r="I46" t="n">
         <v>53.78289216121269</v>
       </c>
+      <c r="J46" t="n">
+        <v>58668</v>
+      </c>
+      <c r="K46" t="n">
+        <v>383146</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1905,6 +2185,12 @@
       <c r="I47" t="n">
         <v>53.8900730081881</v>
       </c>
+      <c r="J47" t="n">
+        <v>27066</v>
+      </c>
+      <c r="K47" t="n">
+        <v>414748</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1936,6 +2222,12 @@
       <c r="I48" t="n">
         <v>55.59543022169371</v>
       </c>
+      <c r="J48" t="n">
+        <v>17986</v>
+      </c>
+      <c r="K48" t="n">
+        <v>423828</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1967,6 +2259,12 @@
       <c r="I49" t="n">
         <v>54.36674092726573</v>
       </c>
+      <c r="J49" t="n">
+        <v>28405</v>
+      </c>
+      <c r="K49" t="n">
+        <v>413409</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1998,6 +2296,12 @@
       <c r="I50" t="n">
         <v>53.90037760265282</v>
       </c>
+      <c r="J50" t="n">
+        <v>46160</v>
+      </c>
+      <c r="K50" t="n">
+        <v>395654</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2029,6 +2333,12 @@
       <c r="I51" t="n">
         <v>53.32567225925074</v>
       </c>
+      <c r="J51" t="n">
+        <v>71979</v>
+      </c>
+      <c r="K51" t="n">
+        <v>369835</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2060,6 +2370,12 @@
       <c r="I52" t="n">
         <v>54.75552190424361</v>
       </c>
+      <c r="J52" t="n">
+        <v>19179</v>
+      </c>
+      <c r="K52" t="n">
+        <v>422635</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2091,6 +2407,12 @@
       <c r="I53" t="n">
         <v>57.2863604990103</v>
       </c>
+      <c r="J53" t="n">
+        <v>91200</v>
+      </c>
+      <c r="K53" t="n">
+        <v>350614</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2122,6 +2444,12 @@
       <c r="I54" t="n">
         <v>55.44816389602705</v>
       </c>
+      <c r="J54" t="n">
+        <v>32823</v>
+      </c>
+      <c r="K54" t="n">
+        <v>408991</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2153,6 +2481,12 @@
       <c r="I55" t="n">
         <v>52.9505289878896</v>
       </c>
+      <c r="J55" t="n">
+        <v>70728</v>
+      </c>
+      <c r="K55" t="n">
+        <v>371086</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2184,6 +2518,12 @@
       <c r="I56" t="n">
         <v>53.88615931423792</v>
       </c>
+      <c r="J56" t="n">
+        <v>20910</v>
+      </c>
+      <c r="K56" t="n">
+        <v>420904</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2215,6 +2555,12 @@
       <c r="I57" t="n">
         <v>54.61851244080405</v>
       </c>
+      <c r="J57" t="n">
+        <v>14631</v>
+      </c>
+      <c r="K57" t="n">
+        <v>427183</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2246,6 +2592,12 @@
       <c r="I58" t="n">
         <v>54.62996084381459</v>
       </c>
+      <c r="J58" t="n">
+        <v>25277</v>
+      </c>
+      <c r="K58" t="n">
+        <v>416537</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2277,6 +2629,12 @@
       <c r="I59" t="n">
         <v>54.73443138596479</v>
       </c>
+      <c r="J59" t="n">
+        <v>20887</v>
+      </c>
+      <c r="K59" t="n">
+        <v>420927</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2308,6 +2666,12 @@
       <c r="I60" t="n">
         <v>53.28615364757222</v>
       </c>
+      <c r="J60" t="n">
+        <v>38957</v>
+      </c>
+      <c r="K60" t="n">
+        <v>402857</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2339,6 +2703,12 @@
       <c r="I61" t="n">
         <v>55.34841142408765</v>
       </c>
+      <c r="J61" t="n">
+        <v>28897</v>
+      </c>
+      <c r="K61" t="n">
+        <v>412917</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2370,6 +2740,12 @@
       <c r="I62" t="n">
         <v>53.58304026801899</v>
       </c>
+      <c r="J62" t="n">
+        <v>27515</v>
+      </c>
+      <c r="K62" t="n">
+        <v>414299</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2401,6 +2777,12 @@
       <c r="I63" t="n">
         <v>53.05985806551418</v>
       </c>
+      <c r="J63" t="n">
+        <v>28102</v>
+      </c>
+      <c r="K63" t="n">
+        <v>413712</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2432,6 +2814,12 @@
       <c r="I64" t="n">
         <v>54.25376518664953</v>
       </c>
+      <c r="J64" t="n">
+        <v>42697</v>
+      </c>
+      <c r="K64" t="n">
+        <v>399117</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2463,6 +2851,12 @@
       <c r="I65" t="n">
         <v>53.22168842695373</v>
       </c>
+      <c r="J65" t="n">
+        <v>21553</v>
+      </c>
+      <c r="K65" t="n">
+        <v>420261</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2494,6 +2888,12 @@
       <c r="I66" t="n">
         <v>54.29657813082392</v>
       </c>
+      <c r="J66" t="n">
+        <v>28648</v>
+      </c>
+      <c r="K66" t="n">
+        <v>413166</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2525,6 +2925,12 @@
       <c r="I67" t="n">
         <v>53.36803187269656</v>
       </c>
+      <c r="J67" t="n">
+        <v>100205</v>
+      </c>
+      <c r="K67" t="n">
+        <v>341609</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2556,6 +2962,12 @@
       <c r="I68" t="n">
         <v>54.03716208284224</v>
       </c>
+      <c r="J68" t="n">
+        <v>15896</v>
+      </c>
+      <c r="K68" t="n">
+        <v>425918</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2587,6 +2999,12 @@
       <c r="I69" t="n">
         <v>54.20160408312067</v>
       </c>
+      <c r="J69" t="n">
+        <v>13906</v>
+      </c>
+      <c r="K69" t="n">
+        <v>427908</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2618,6 +3036,12 @@
       <c r="I70" t="n">
         <v>54.19739284725284</v>
       </c>
+      <c r="J70" t="n">
+        <v>51810</v>
+      </c>
+      <c r="K70" t="n">
+        <v>390004</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2649,6 +3073,12 @@
       <c r="I71" t="n">
         <v>53.8382165390114</v>
       </c>
+      <c r="J71" t="n">
+        <v>27025</v>
+      </c>
+      <c r="K71" t="n">
+        <v>414789</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2680,6 +3110,12 @@
       <c r="I72" t="n">
         <v>52.62361914781694</v>
       </c>
+      <c r="J72" t="n">
+        <v>15990</v>
+      </c>
+      <c r="K72" t="n">
+        <v>425824</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2711,6 +3147,12 @@
       <c r="I73" t="n">
         <v>54.95473836567475</v>
       </c>
+      <c r="J73" t="n">
+        <v>34184</v>
+      </c>
+      <c r="K73" t="n">
+        <v>407630</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2742,6 +3184,12 @@
       <c r="I74" t="n">
         <v>53.41907293657348</v>
       </c>
+      <c r="J74" t="n">
+        <v>21627</v>
+      </c>
+      <c r="K74" t="n">
+        <v>420187</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2773,6 +3221,12 @@
       <c r="I75" t="n">
         <v>53.12080969083568</v>
       </c>
+      <c r="J75" t="n">
+        <v>45811</v>
+      </c>
+      <c r="K75" t="n">
+        <v>396003</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2804,6 +3258,12 @@
       <c r="I76" t="n">
         <v>54.32959411161045</v>
       </c>
+      <c r="J76" t="n">
+        <v>46188</v>
+      </c>
+      <c r="K76" t="n">
+        <v>395626</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2835,6 +3295,12 @@
       <c r="I77" t="n">
         <v>52.52704578353939</v>
       </c>
+      <c r="J77" t="n">
+        <v>39071</v>
+      </c>
+      <c r="K77" t="n">
+        <v>402743</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2866,6 +3332,12 @@
       <c r="I78" t="n">
         <v>53.93233340509852</v>
       </c>
+      <c r="J78" t="n">
+        <v>65587</v>
+      </c>
+      <c r="K78" t="n">
+        <v>376227</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2897,6 +3369,12 @@
       <c r="I79" t="n">
         <v>54.62109270975032</v>
       </c>
+      <c r="J79" t="n">
+        <v>24997</v>
+      </c>
+      <c r="K79" t="n">
+        <v>416817</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2928,6 +3406,12 @@
       <c r="I80" t="n">
         <v>53.82671678450637</v>
       </c>
+      <c r="J80" t="n">
+        <v>59515</v>
+      </c>
+      <c r="K80" t="n">
+        <v>382299</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2959,6 +3443,12 @@
       <c r="I81" t="n">
         <v>56.67666329431034</v>
       </c>
+      <c r="J81" t="n">
+        <v>109702</v>
+      </c>
+      <c r="K81" t="n">
+        <v>332112</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2990,6 +3480,12 @@
       <c r="I82" t="n">
         <v>56.37035496225238</v>
       </c>
+      <c r="J82" t="n">
+        <v>33179</v>
+      </c>
+      <c r="K82" t="n">
+        <v>408635</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3021,6 +3517,12 @@
       <c r="I83" t="n">
         <v>54.55342037491474</v>
       </c>
+      <c r="J83" t="n">
+        <v>29827</v>
+      </c>
+      <c r="K83" t="n">
+        <v>411987</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3052,6 +3554,12 @@
       <c r="I84" t="n">
         <v>54.20960557102794</v>
       </c>
+      <c r="J84" t="n">
+        <v>28533</v>
+      </c>
+      <c r="K84" t="n">
+        <v>413281</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3083,6 +3591,12 @@
       <c r="I85" t="n">
         <v>53.55547463843136</v>
       </c>
+      <c r="J85" t="n">
+        <v>21631</v>
+      </c>
+      <c r="K85" t="n">
+        <v>420183</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3114,6 +3628,12 @@
       <c r="I86" t="n">
         <v>54.82457617739196</v>
       </c>
+      <c r="J86" t="n">
+        <v>26192</v>
+      </c>
+      <c r="K86" t="n">
+        <v>415622</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3145,6 +3665,12 @@
       <c r="I87" t="n">
         <v>53.5326285825323</v>
       </c>
+      <c r="J87" t="n">
+        <v>45551</v>
+      </c>
+      <c r="K87" t="n">
+        <v>396263</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3176,6 +3702,12 @@
       <c r="I88" t="n">
         <v>56.2978111234203</v>
       </c>
+      <c r="J88" t="n">
+        <v>60888</v>
+      </c>
+      <c r="K88" t="n">
+        <v>380926</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3207,6 +3739,12 @@
       <c r="I89" t="n">
         <v>56.55014584864941</v>
       </c>
+      <c r="J89" t="n">
+        <v>20144</v>
+      </c>
+      <c r="K89" t="n">
+        <v>421670</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3238,6 +3776,12 @@
       <c r="I90" t="n">
         <v>54.58284299153131</v>
       </c>
+      <c r="J90" t="n">
+        <v>34785</v>
+      </c>
+      <c r="K90" t="n">
+        <v>407029</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3269,6 +3813,12 @@
       <c r="I91" t="n">
         <v>53.80637727340621</v>
       </c>
+      <c r="J91" t="n">
+        <v>20035</v>
+      </c>
+      <c r="K91" t="n">
+        <v>421779</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3300,6 +3850,12 @@
       <c r="I92" t="n">
         <v>52.4027282966515</v>
       </c>
+      <c r="J92" t="n">
+        <v>28076</v>
+      </c>
+      <c r="K92" t="n">
+        <v>413738</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3331,6 +3887,12 @@
       <c r="I93" t="n">
         <v>54.03710434614845</v>
       </c>
+      <c r="J93" t="n">
+        <v>21971</v>
+      </c>
+      <c r="K93" t="n">
+        <v>419843</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3362,6 +3924,12 @@
       <c r="I94" t="n">
         <v>52.44963547255811</v>
       </c>
+      <c r="J94" t="n">
+        <v>80250</v>
+      </c>
+      <c r="K94" t="n">
+        <v>361564</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3393,6 +3961,12 @@
       <c r="I95" t="n">
         <v>55.24809208308808</v>
       </c>
+      <c r="J95" t="n">
+        <v>44260</v>
+      </c>
+      <c r="K95" t="n">
+        <v>397554</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3424,6 +3998,12 @@
       <c r="I96" t="n">
         <v>54.21106926200893</v>
       </c>
+      <c r="J96" t="n">
+        <v>27893</v>
+      </c>
+      <c r="K96" t="n">
+        <v>413921</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3455,6 +4035,12 @@
       <c r="I97" t="n">
         <v>53.97253108488778</v>
       </c>
+      <c r="J97" t="n">
+        <v>25052</v>
+      </c>
+      <c r="K97" t="n">
+        <v>416762</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3486,6 +4072,12 @@
       <c r="I98" t="n">
         <v>54.18030886912179</v>
       </c>
+      <c r="J98" t="n">
+        <v>27658</v>
+      </c>
+      <c r="K98" t="n">
+        <v>414156</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3517,6 +4109,12 @@
       <c r="I99" t="n">
         <v>55.52245563419797</v>
       </c>
+      <c r="J99" t="n">
+        <v>26573</v>
+      </c>
+      <c r="K99" t="n">
+        <v>415241</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3548,6 +4146,12 @@
       <c r="I100" t="n">
         <v>53.90726187403659</v>
       </c>
+      <c r="J100" t="n">
+        <v>19485</v>
+      </c>
+      <c r="K100" t="n">
+        <v>422329</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3579,6 +4183,12 @@
       <c r="I101" t="n">
         <v>54.50835791543756</v>
       </c>
+      <c r="J101" t="n">
+        <v>14674</v>
+      </c>
+      <c r="K101" t="n">
+        <v>427140</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3610,6 +4220,12 @@
       <c r="I102" t="n">
         <v>54.71260485010539</v>
       </c>
+      <c r="J102" t="n">
+        <v>21452</v>
+      </c>
+      <c r="K102" t="n">
+        <v>420362</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3641,6 +4257,12 @@
       <c r="I103" t="n">
         <v>54.11995231181464</v>
       </c>
+      <c r="J103" t="n">
+        <v>18229</v>
+      </c>
+      <c r="K103" t="n">
+        <v>423585</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3672,6 +4294,12 @@
       <c r="I104" t="n">
         <v>54.00288359386857</v>
       </c>
+      <c r="J104" t="n">
+        <v>20118</v>
+      </c>
+      <c r="K104" t="n">
+        <v>421696</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3703,6 +4331,12 @@
       <c r="I105" t="n">
         <v>53.78233463238563</v>
       </c>
+      <c r="J105" t="n">
+        <v>59484</v>
+      </c>
+      <c r="K105" t="n">
+        <v>382330</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3734,6 +4368,12 @@
       <c r="I106" t="n">
         <v>54.51896804555327</v>
       </c>
+      <c r="J106" t="n">
+        <v>27881</v>
+      </c>
+      <c r="K106" t="n">
+        <v>413933</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3765,6 +4405,12 @@
       <c r="I107" t="n">
         <v>54.34714036689632</v>
       </c>
+      <c r="J107" t="n">
+        <v>20169</v>
+      </c>
+      <c r="K107" t="n">
+        <v>421645</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3796,6 +4442,12 @@
       <c r="I108" t="n">
         <v>53.83486325689653</v>
       </c>
+      <c r="J108" t="n">
+        <v>20769</v>
+      </c>
+      <c r="K108" t="n">
+        <v>421045</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3827,6 +4479,12 @@
       <c r="I109" t="n">
         <v>54.18664081996658</v>
       </c>
+      <c r="J109" t="n">
+        <v>41505</v>
+      </c>
+      <c r="K109" t="n">
+        <v>400309</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3857,6 +4515,12 @@
       </c>
       <c r="I110" t="n">
         <v>55.33224041895581</v>
+      </c>
+      <c r="J110" t="n">
+        <v>21531</v>
+      </c>
+      <c r="K110" t="n">
+        <v>420283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>